<commit_message>
Update Projeto controle de investimentos
Alteração na visibilidade do arquivo para uma forma mais ampla. Células protegidas.
</commit_message>
<xml_diff>
--- a/Projeto controle de investimentos.xlsx
+++ b/Projeto controle de investimentos.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jc_ba\Documents\DIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E23F1B8-8679-4A89-BAEC-F26CF7499BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31498B55-DAEA-4CAF-85EB-8E05E8C0BA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha3" sheetId="4" r:id="rId1"/>
+    <sheet name="Planilha3" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Plan1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -260,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +295,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -464,11 +470,86 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,89 +563,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -584,24 +593,6 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="2" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -738,6 +729,24 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1042,8 +1051,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1133,6 +1141,62 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1166,6 +1230,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6CEB-47A0-9565-46F244171CDD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1181,6 +1250,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6CEB-47A0-9565-46F244171CDD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1196,6 +1270,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6CEB-47A0-9565-46F244171CDD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1211,6 +1290,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6CEB-47A0-9565-46F244171CDD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1295,16 +1379,16 @@
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>46827.240159688023</c:v>
+                  <c:v>92026.445663584993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63532.2689637609</c:v>
+                  <c:v>217005.19598118198</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31815.937233928031</c:v>
+                  <c:v>83506.206134794818</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20693.964817155651</c:v>
+                  <c:v>93088.968114149437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2034,8 +2118,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="PERÍODO">
@@ -2058,7 +2142,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2187,7 +2271,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7BC9E95-A67E-4607-8143-F6E8BD6BE180}" name="Tabela dinâmica5" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7BC9E95-A67E-4607-8143-F6E8BD6BE180}" name="Tabela dinâmica5" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" outline="0" showAll="0" defaultSubtotal="0">
@@ -2226,7 +2310,7 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="0" item="1" hier="-1"/>
+    <pageField fld="0" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="4">
     <dataField name="  INVESTIMENTO 1" fld="1" baseField="0" baseItem="0" numFmtId="44"/>
@@ -2234,7 +2318,7 @@
     <dataField name="  INVESTIMENTO 3" fld="3" baseField="0" baseItem="0" numFmtId="44"/>
     <dataField name="  INVESTIMENTO 4" fld="4" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
-  <chartFormats count="4">
+  <chartFormats count="8">
     <chartFormat chart="3" format="13" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -2271,6 +2355,42 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="3" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="19">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2294,8 +2414,8 @@
       <items count="5">
         <i x="0"/>
         <i x="1"/>
-        <i x="2" s="1"/>
-        <i x="3"/>
+        <i x="2"/>
+        <i x="3" s="1"/>
         <i x="4"/>
       </items>
     </tabular>
@@ -2310,28 +2430,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2DB16D87-43B8-42ED-82E0-CE3F5FBFE35F}" name="Tabela2" displayName="Tabela2" ref="A11:F16" totalsRowShown="0" dataDxfId="1" tableBorderDxfId="8" dataCellStyle="Moeda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2DB16D87-43B8-42ED-82E0-CE3F5FBFE35F}" name="Tabela2" displayName="Tabela2" ref="A11:F16" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7" dataCellStyle="Moeda">
   <autoFilter ref="A11:F16" xr:uid="{2DB16D87-43B8-42ED-82E0-CE3F5FBFE35F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:F16">
     <sortCondition ref="A12:A16" customList="1 ANO,5 ANOS,10 ANOS,15 ANOS,20 ANOS"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AD1347C-ED74-40E9-BF80-96CDE483B0B5}" name="PERÍODO" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{1AD1347C-ED74-40E9-BF80-96CDE483B0B5}" name="PERÍODO" dataDxfId="6">
       <calculatedColumnFormula>Plan1!B20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{DF2ECC2A-1C0C-4F9E-A83D-133B93D44820}" name="INVESTIMENTO 1" dataDxfId="6" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{DF2ECC2A-1C0C-4F9E-A83D-133B93D44820}" name="INVESTIMENTO 1" dataDxfId="5" dataCellStyle="Moeda">
       <calculatedColumnFormula>Plan1!C20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{775E285C-1023-44C4-B1E7-EDD8F4BB76C7}" name="INVESTIMENTO 2" dataDxfId="5" dataCellStyle="Moeda">
+    <tableColumn id="3" xr3:uid="{775E285C-1023-44C4-B1E7-EDD8F4BB76C7}" name="INVESTIMENTO 2" dataDxfId="4" dataCellStyle="Moeda">
       <calculatedColumnFormula>Plan1!D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4394707B-E890-4E49-91D6-DBFBB386927D}" name="INVESTIMENTO 3" dataDxfId="4" dataCellStyle="Moeda">
+    <tableColumn id="4" xr3:uid="{4394707B-E890-4E49-91D6-DBFBB386927D}" name="INVESTIMENTO 3" dataDxfId="3" dataCellStyle="Moeda">
       <calculatedColumnFormula>Plan1!E20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{66265B92-76DB-407B-AD59-B1743F398106}" name="INVESTIMENTO 4" dataDxfId="3" dataCellStyle="Moeda">
+    <tableColumn id="5" xr3:uid="{66265B92-76DB-407B-AD59-B1743F398106}" name="INVESTIMENTO 4" dataDxfId="2" dataCellStyle="Moeda">
       <calculatedColumnFormula>Plan1!F20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F0A1C77D-A21A-4158-8AC0-823C7025F9D2}" name="TOTAIS" dataDxfId="2" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{F0A1C77D-A21A-4158-8AC0-823C7025F9D2}" name="TOTAIS" dataDxfId="1" dataCellStyle="Moeda">
       <calculatedColumnFormula>Plan1!G20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2611,22 +2731,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2635,7 +2755,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="1">
-        <v>46827.240159688023</v>
+        <v>92026.445663584993</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2643,7 +2763,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="1">
-        <v>63532.2689637609</v>
+        <v>217005.19598118198</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2651,7 +2771,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>31815.937233928031</v>
+        <v>83506.206134794818</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2659,7 +2779,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>20693.964817155651</v>
+        <v>93088.968114149437</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2683,131 +2803,131 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="str">
+      <c r="A12" s="15" t="str">
         <f>Plan1!B20</f>
         <v>1 ANO</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="11">
         <f>Plan1!C20</f>
         <v>7459.376290727806</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="11">
         <f>Plan1!D20</f>
         <v>4176.5112160159078</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="11">
         <f>Plan1!E20</f>
         <v>3173.7090287691994</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="11">
         <f>Plan1!F20</f>
         <v>879.37770667092718</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="12">
         <f>Plan1!G20</f>
         <v>15688.974242183842</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="str">
+      <c r="A13" s="15" t="str">
         <f>Plan1!B21</f>
         <v>5 ANOS</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="11">
         <f>Plan1!C21</f>
         <v>20423.781087047744</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="11">
         <f>Plan1!D21</f>
         <v>16756.442427283815</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="11">
         <f>Plan1!E21</f>
         <v>10659.318654138333</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="11">
         <f>Plan1!F21</f>
         <v>4239.7687236965376</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="12">
         <f>Plan1!G21</f>
         <v>52079.310892166432</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="str">
+      <c r="A14" s="15" t="str">
         <f>Plan1!B22</f>
         <v>10 ANOS</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="11">
         <f>Plan1!C22</f>
         <v>46827.240159688023</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="11">
         <f>Plan1!D22</f>
         <v>63532.2689637609</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="11">
         <f>Plan1!E22</f>
         <v>31815.937233928031</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="11">
         <f>Plan1!F22</f>
         <v>20693.964817155651</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="12">
         <f>Plan1!G22</f>
         <v>162869.41117453261</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="str">
+      <c r="A15" s="15" t="str">
         <f>Plan1!B23</f>
         <v>15 ANOS</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="11">
         <f>Plan1!C23</f>
         <v>92026.445663584993</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="11">
         <f>Plan1!D23</f>
         <v>217005.19598118198</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="11">
         <f>Plan1!E23</f>
         <v>83506.206134794818</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="11">
         <f>Plan1!F23</f>
         <v>93088.968114149437</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="12">
         <f>Plan1!G23</f>
         <v>485626.81589371117</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="str">
+      <c r="A16" s="15" t="str">
         <f>Plan1!B24</f>
         <v>20 ANOS</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="11">
         <f>Plan1!C24</f>
         <v>169401.46582904761</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="11">
         <f>Plan1!D24</f>
         <v>720554.59470589808</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="11">
         <f>Plan1!E24</f>
         <v>209796.89332411202</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="11">
         <f>Plan1!F24</f>
         <v>411611.76148569328</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="12">
         <f>Plan1!G24</f>
         <v>1511364.715344751</v>
       </c>
@@ -2822,424 +2942,418 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G32"/>
+  <dimension ref="A2:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="19.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="12" hidden="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="21">
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="28">
         <v>10000</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="21">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="28">
         <v>300</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="35"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="26">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="26">
         <v>0.02</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="26">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="26">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G12" s="35"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="27">
         <v>0.5</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="27">
         <v>0.25</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="27">
         <v>0.2</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="27">
         <v>0.05</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="11">
         <f>$G$8*C13</f>
         <v>5000</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="11">
         <f>$G$8*D13</f>
         <v>2500</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="11">
         <f>$G$8*E13</f>
         <v>2000</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="11">
         <f>$G$8*F13</f>
         <v>500</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="12">
         <f t="shared" ref="G17:G18" si="0">SUM(C17:F17)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="11">
         <f>$G$9*C13</f>
         <v>150</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="11">
         <f>$G$9*D13</f>
         <v>75</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="11">
         <f>$G$9*E13</f>
         <v>60</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="11">
         <f>$G$9*F13</f>
         <v>15</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="12">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="11">
         <f>FV(C$12,12,-C$18,-C$17,)</f>
         <v>7459.376290727806</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="11">
         <f>FV(D12,12,-D$18,-D$17,)</f>
         <v>4176.5112160159078</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="11">
         <f>FV(E12,12,-E$18,-E$17,)</f>
         <v>3173.7090287691994</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="11">
         <f>FV(F12,12,-F$18,-F$17,)</f>
         <v>879.37770667092718</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="12">
         <f>SUM(C20:F20)</f>
         <v>15688.974242183842</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="11">
         <f>FV(C$12,12*5,-C$18,-C$17,)</f>
         <v>20423.781087047744</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="11">
         <f>FV(D$12,12*5,-D$18,-D$17,)</f>
         <v>16756.442427283815</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="11">
         <f>FV(E$12,12*5,-E$18,-E$17,)</f>
         <v>10659.318654138333</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="11">
         <f>FV(F$12,12*5,-F$18,-F$17,)</f>
         <v>4239.7687236965376</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="12">
         <f t="shared" ref="G21:G24" si="1">SUM(C21:F21)</f>
         <v>52079.310892166432</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="11">
         <f>FV(C$12,12*10,-C$18,-C$17,)</f>
         <v>46827.240159688023</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="11">
         <f>FV(D$12,12*10,-D$18,-D$17,)</f>
         <v>63532.2689637609</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="11">
         <f>FV(E$12,12*10,-E$18,-E$17,)</f>
         <v>31815.937233928031</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="11">
         <f>FV(F$12,12*10,-F$18,-F$17,)</f>
         <v>20693.964817155651</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="12">
         <f t="shared" si="1"/>
         <v>162869.41117453261</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="11">
         <f>FV(C$12,12*15,-C$18,-C$17,)</f>
         <v>92026.445663584993</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="11">
         <f>FV(D$12,12*15,-D$18,-D$17,)</f>
         <v>217005.19598118198</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="11">
         <f>FV(E$12,12*15,-E$18,-E$17,)</f>
         <v>83506.206134794818</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="11">
         <f>FV(F$12,12*15,-F$18,-F$17,)</f>
         <v>93088.968114149437</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="12">
         <f t="shared" si="1"/>
         <v>485626.81589371117</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="13">
         <f>FV(C$12,12*20,-C$18,-C$17,)</f>
         <v>169401.46582904761</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="13">
         <f>FV(D$12,12*20,-D$18,-D$17,)</f>
         <v>720554.59470589808</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="13">
         <f>FV(E$12,12*20,-E$18,-E$17,)</f>
         <v>209796.89332411202</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="13">
         <f>FV(F$12,12*20,-F$18,-F$17,)</f>
         <v>411611.76148569328</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="14">
         <f t="shared" si="1"/>
         <v>1511364.715344751</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="46"/>
+      <c r="D26" s="34"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27"/>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="39">
+      <c r="D27" s="20">
         <f>$C$12*GETPIVOTDATA("  INVESTIMENTO 1",Planilha3!$B$4)</f>
-        <v>421.44516143719216</v>
+        <v>828.23801097226487</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28"/>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="40">
+      <c r="D28" s="21">
         <f>$D$12*GETPIVOTDATA("  INVESTIMENTO 2",Planilha3!$A$3)</f>
-        <v>1270.6453792752179</v>
+        <v>4340.1039196236397</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29"/>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="39">
+      <c r="D29" s="20">
         <f>$E$12*GETPIVOTDATA("  INVESTIMENTO 3",Planilha3!$A$3)</f>
-        <v>477.23905850892044</v>
+        <v>1252.5930920219223</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30"/>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="40">
+      <c r="D30" s="21">
         <f>$F$12*GETPIVOTDATA("  INVESTIMENTO 4",Planilha3!$A$3)</f>
-        <v>517.3491204288913</v>
+        <v>2327.2242028537362</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31"/>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="22">
         <f>SUM(D27:D30)</f>
-        <v>2686.6787196502219</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32"/>
-    </row>
+        <v>8748.1592254715633</v>
+      </c>
+    </row>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="9">
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B2:G2"/>

</xml_diff>